<commit_message>
updated answers for week 2, change difference in rank to be positive for lower rank
</commit_message>
<xml_diff>
--- a/external-files/answer_truth.xlsx
+++ b/external-files/answer_truth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeague/external-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18585A36-B07F-1D44-A9D8-EA52263DF613}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D31A54-5AD8-0C43-868D-AA5741BCE483}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="3060" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>question</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>None of the above</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1042,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,10 +1722,13 @@
         <v>3</v>
       </c>
       <c r="C43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
some results week over week
</commit_message>
<xml_diff>
--- a/external-files/answer_truth.xlsx
+++ b/external-files/answer_truth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annes/Documents/Personal/GoT/GameOfThronesLeague/external-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D31A54-5AD8-0C43-868D-AA5741BCE483}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D82B06F-6893-BF40-9F8D-2A580F1DEC2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="3060" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="answer_structure" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>question</t>
   </si>
@@ -191,6 +191,27 @@
   </si>
   <si>
     <t>None of the above</t>
+  </si>
+  <si>
+    <t>Dies</t>
+  </si>
+  <si>
+    <t>Arya Stark</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Edd Tollett</t>
+  </si>
+  <si>
+    <t>Rhaegal</t>
+  </si>
+  <si>
+    <t>Arya kills the Knight's King</t>
+  </si>
+  <si>
+    <t>The Hound kills Ser Gregor, Ser Gregor kills Qyburn</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1235,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1252,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1286,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1320,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1371,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1388,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1439,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1495,10 +1516,13 @@
         <v>5</v>
       </c>
       <c r="C27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1509,10 +1533,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1537,10 +1564,13 @@
         <v>4</v>
       </c>
       <c r="C30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,10 +1581,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1565,10 +1598,13 @@
         <v>1</v>
       </c>
       <c r="C32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1579,10 +1615,13 @@
         <v>1</v>
       </c>
       <c r="C33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1593,10 +1632,13 @@
         <v>1</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1621,10 +1663,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1635,10 +1680,13 @@
         <v>1</v>
       </c>
       <c r="C37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="b">
         <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1652,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1666,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1680,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40" t="s">
         <v>55</v>
@@ -1697,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1753,10 +1801,13 @@
         <v>2</v>
       </c>
       <c r="C45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1767,10 +1818,13 @@
         <v>2</v>
       </c>
       <c r="C46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1822,8 +1876,14 @@
       <c r="C50" t="b">
         <v>0</v>
       </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
+    <sortCondition ref="A2:A50"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>